<commit_message>
Xiling's final diary update
</commit_message>
<xml_diff>
--- a/diaries/diary-xiling-li.xlsx
+++ b/diaries/diary-xiling-li.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lixiling/Documents/UCI/courses/265p/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E51DDC-645A-DD4F-85B7-6B7E2190E5DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB354620-A72C-F54D-8EA1-5862BC502993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28020" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="107">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Learned different styles and discovered my own preference</t>
   </si>
   <si>
-    <t>Listening to other students' reading strategy surprised me, because it is so different from me. I thought, 'Very organised thinking, but why bother that much of rest of the code?' Then I am happy I volunteered to try reading code during class. Because of that my learning experience enhanced. Thinking out loud made me realized clearly what my reading strategy is, and the benefit of other's strategy. And I enjoyed the guest talk. Made me realize that I should do more research into the industry.</t>
-  </si>
-  <si>
     <t xml:space="preserve">I enjoyed it all the way, I cannot thinking  of ditching any part of the class. </t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Both done.</t>
   </si>
   <si>
-    <t>I spend almost whole day trying to finish all the homework. Reading code is still not easy to me. During the code reading I gradually refined my reading strategy, I lowered my intent to do opportunistic comprehension and do more systematic comprehension. I think things work out better. After created a wrong pull request I spent some time learning more about Git &amp; Github. I found a video on youtube which is quite helpful.</t>
-  </si>
-  <si>
     <t>Jan 29 2020</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Lesson</t>
   </si>
   <si>
-    <t>Seems like all projects we chose have a somewhat similar UML.(some super long lines at first, and scattered chuncks)</t>
-  </si>
-  <si>
     <t>This is the first time that our team actually work together. Interestingly that every person starts to act in different roles. Will see if the roles will be consistent in the future.</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>Working on hw2</t>
   </si>
   <si>
-    <t>Two essential features are analysed</t>
-  </si>
-  <si>
     <t>Foobar team &amp; myself</t>
   </si>
   <si>
@@ -231,15 +219,9 @@
     <t>good, tired</t>
   </si>
   <si>
-    <t xml:space="preserve">Continuing yesterday's feeling, I found that I cannot understand some of the questions precisely. Terms such as implemetation, abstraction, although I know what they mean, but I don’t what exactly is the meaning in certain scenarios. </t>
-  </si>
-  <si>
     <t>Feels good to catch up what I left behind.</t>
   </si>
   <si>
-    <t>Remembered a lot if terms</t>
-  </si>
-  <si>
     <t>Understanding more about the social context of an big open source project and what contributors expect from the repo owner.</t>
   </si>
   <si>
@@ -252,16 +234,118 @@
     <t>Design Pattern</t>
   </si>
   <si>
-    <t>During the past few days I was learning design patterns, A LOT of design patterns. After 2 round learning I start to find some patterns in the repo and luckily I did find some. And it also proved that the patterns are really useful because some patterns can be identified just by  the names classes are using. But still, with suddenly 23 patterns in my head, I should spend more time later to better remember and distinguish them.</t>
-  </si>
-  <si>
     <t>Got a sense of what each design pattern is talking about.</t>
   </si>
   <si>
     <t>final's pressure is coming…</t>
   </si>
   <si>
-    <t>It was a very interesting experience to figure out the architecture of Telegram together. We made quite a lot of assumption but got stuck or confused in the middle quite a few times. And as the Telegram website has massivce information but lack of organization, it also took us quite a lot of time to search for useful information on Telegram as well as other technical news websites to summarize what we found.</t>
+    <t>During the past few days I was learning design patterns, A LOT of design patterns. After 2 round learning I start to look for some patterns in the repo and luckily I did find some. And it also proved that the patterns are really useful because some patterns can be identified just by  the names classes are using. But still, with suddenly 23 patterns in my head, I should spend more time later to better remember and distinguish them.</t>
+  </si>
+  <si>
+    <t>March 5 2020</t>
+  </si>
+  <si>
+    <t>hw5</t>
+  </si>
+  <si>
+    <t>found patterns and described them</t>
+  </si>
+  <si>
+    <t>March 11 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starting hw6 </t>
+  </si>
+  <si>
+    <t>March 13 2020</t>
+  </si>
+  <si>
+    <t>continuing hw6</t>
+  </si>
+  <si>
+    <t>March 12 2020</t>
+  </si>
+  <si>
+    <t>March 7 2020</t>
+  </si>
+  <si>
+    <t>rewrite hw3</t>
+  </si>
+  <si>
+    <t>March 17 2020</t>
+  </si>
+  <si>
+    <t>good - looking forward to the challenges ahead</t>
+  </si>
+  <si>
+    <t>good - it's always good to learn new things, and when  tasks have even teeny tiny progress, I feel contented.</t>
+  </si>
+  <si>
+    <t>When I was trying to write some test cases, I realized I am doing something that I have never done before: I have to create the testing environment and design the test cases from scratch. So I spent a lot of time to learn testing of Android.</t>
+  </si>
+  <si>
+    <t>Listening to other students' reading strategy surprised me, because it is so different from me. I thought, 'Very organized thinking, but why bother that much of rest of the code?' Then I am happy I volunteered to try reading code during class. Because of that my learning experience enhanced. Thinking out loud made me realized clearly what my reading strategy is, and the benefit of other's strategy. And I enjoyed the guest talk. Made me realize that I should do more research into the industry.</t>
+  </si>
+  <si>
+    <t>I spend almost whole day trying to finish all the homework. Reading code is still not easy to me. During the code reading I gradually refined my reading strategy, I lowered my intent to do opportunistic comprehension and do more systematic comprehension. I think things work out better. After created a wrong pull request I spent some time learning more about Git &amp; GitHub. I found a video on YouTube which is quite helpful.</t>
+  </si>
+  <si>
+    <t>Seems like all projects we chose have a somewhat similar UML.(some super long lines at first, and scattered chunks)</t>
+  </si>
+  <si>
+    <t>Two essential features are analyzed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuing yesterday's feeling, I found that I cannot understand some of the questions precisely. Terms such as implementation, abstraction, although I know what they mean, but I don’t what exactly is the meaning in certain scenarios. </t>
+  </si>
+  <si>
+    <t>It was a very interesting experience to figure out the architecture of Telegram together. We made quite a lot of assumption but got stuck or confused in the middle quite a few times. And as the Telegram website has massive information but lack of organization, it also took us quite a lot of time to search for useful information on Telegram as well as other technical news websites to summarize what we found.</t>
+  </si>
+  <si>
+    <t>Although I though I found some patterns before, when actually digging into how the patterns work, it is still not an easy task to me. I feel like time is too short to understand all the patterns thoroughly, not mentioning to actually identify them confidently in source code. I just have to say I tried my best.</t>
+  </si>
+  <si>
+    <t>I enjoy look at the same problem from a different perspective. This time is about the test cases. Now I learned a new way to understand a system.</t>
+  </si>
+  <si>
+    <t>We spent more than half hour with Kaj during his office hour to determine how to improve our hw3's hideous score. He is very patient trying to help us figure out what is missing and unclear in our report and we are much more confident to revise our report and more clear about the knowledge points. I hope we had done the same thing with hw2. The 10-minute discussion was not so helpful compare to this time. In the future, we would definitely make better use of the resources that is provided to us.</t>
+  </si>
+  <si>
+    <t>As a unique repo, Telegram again didn't disappoint us this time - there is no test cases. There are a few commented out debugging traces though. And as an Android app, I guess there are a lot of alternatives to test the code as what I already know about testing in Java. So I looked up a little bit about Android Testing, but that seems like a big topic, and again a lot of new jargons appear before me.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was sort of a frustrating experience trying to find the functions that are related to our second pull request. We found a lot of fields and methods that seems related to the function, but  we are not so sure about whether they are really what we thought it is. And as for test cases, when developing test cases, as an app that involves a complicated remote database, the dependency is also very hard to handle. We tried our best. However, we all have the feeling that as for the beginning of the quarter, we all can understand the repo much better and not so intimidated about reading the code any more. </t>
+  </si>
+  <si>
+    <t>Remembered a lot of terms</t>
+  </si>
+  <si>
+    <t>Got a better understanding of the whole picture of Telegram.</t>
+  </si>
+  <si>
+    <t>frustrating - hope there is more time to dig deep.</t>
+  </si>
+  <si>
+    <t>good, always happy to learn new things</t>
+  </si>
+  <si>
+    <t>Another good example tells that there are a lot of times the core is more important than its presentation. The dazzling presentations of developing history are beautiful but merely useful, the next few ones are much more useful although they are not so good looking. But interestingly, I realized that for me because of the fancy useless presentations of history made me more interested in what is really useful. In the future I should try to be more focused on the functions when reviewing tools.</t>
+  </si>
+  <si>
+    <t>Good and feel lucky to have this course designed. Although there are a lot of obstacles and drawbacks during writing homework, I learned a lot and are more comfortable and optimistic about what I will be facing in the future.</t>
+  </si>
+  <si>
+    <t>Finished with a lot of changes.</t>
+  </si>
+  <si>
+    <t>Try to understand test related issues with Telegram.</t>
+  </si>
+  <si>
+    <t>Finish the last homework at best try.</t>
+  </si>
+  <si>
+    <t>Learn more about testing.</t>
   </si>
 </sst>
 </file>
@@ -400,7 +484,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -431,6 +515,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -753,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -771,24 +858,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -902,7 +989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="199" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
@@ -917,345 +1004,431 @@
         <v>22</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="8">
         <v>0.97916666666666663</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="8">
         <v>0.95833333333333337</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="G13" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8">
         <v>0.95833333333333337</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="8">
         <v>0.83333333333333337</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="B16" s="8">
         <v>0.66666666666666663</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" s="8">
         <v>0.91666666666666663</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B18" s="8">
         <v>0.91666666666666663</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="8">
         <v>0.91666666666666663</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8">
         <v>0.66666666666666663</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B21" s="8">
         <v>0.91666666666666663</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B22" s="8">
         <v>0.66666666666666663</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="F22" s="6" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B23" s="8">
         <v>0.91666666666666663</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B24" s="8">
         <v>0.91666666666666663</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="E28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="8">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
+      <c r="D30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
@@ -2102,6 +2275,24 @@
       <c r="E125" s="6"/>
       <c r="F125" s="6"/>
       <c r="G125" s="7"/>
+    </row>
+    <row r="126" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="7"/>
+    </row>
+    <row r="127" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>